<commit_message>
subiendo la ultima version del repositorio encontrado en el servidor
</commit_message>
<xml_diff>
--- a/PHPExcel/Examples/Format_CPE_COMPRAS.xlsx
+++ b/PHPExcel/Examples/Format_CPE_COMPRAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\_______2022\QUIROZ\saludmadremujer\PHPExcel\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Sanchez\AppData\Local\Temp\fz3temp-5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4AC5F4-7FFD-44C2-9FA7-FDDD328F04E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724EAFFA-28FE-4609-805F-44A9A556E572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1065" yWindow="-120" windowWidth="37455" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4650" yWindow="3465" windowWidth="20715" windowHeight="11835" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name=" Registro de Ingresos" sheetId="8" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Número correlativo del registro o código</t>
   </si>
@@ -147,9 +147,6 @@
     <t>INGRESOS</t>
   </si>
   <si>
-    <t>COMISION</t>
-  </si>
-  <si>
     <t>Empresa:  </t>
   </si>
   <si>
@@ -165,10 +162,22 @@
     <t>No.</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Reporte de INGRESOS/Comisiones - CLINICA</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>Tarjeta</t>
+  </si>
+  <si>
+    <t>CENTRO MEDICO ESPECIALIZADO SALUD MADRE &amp; MUJER S.A.C.</t>
+  </si>
+  <si>
+    <t>CAL.EL VIRREY NRO. 125 URB. BANCARIOS LAMBAYEQUE - CHICLAYO - CHICLAYO</t>
+  </si>
+  <si>
+    <t>Comisión</t>
   </si>
 </sst>
 </file>
@@ -180,7 +189,7 @@
     <numFmt numFmtId="164" formatCode="000000"/>
     <numFmt numFmtId="165" formatCode="00000000"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -364,6 +373,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color theme="0"/>
       <name val="Arial Narrow"/>
@@ -372,19 +382,43 @@
     <font>
       <b/>
       <sz val="9"/>
-      <color theme="0"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <color theme="1" tint="0.249977111117893"/>
+      <color theme="1"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -421,8 +455,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE598"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -540,6 +580,45 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -555,7 +634,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
@@ -564,8 +643,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -659,7 +739,40 @@
     <xf numFmtId="2" fontId="26" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="25" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="26" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="25" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="29" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="30" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="8" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="33" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="34" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -670,73 +783,55 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="14" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="29" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="30" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="31" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal 2 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -745,6 +840,7 @@
     <cellStyle name="Normal 4 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="Normal 5" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 6" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 7" xfId="8" xr:uid="{54F31630-8F60-4B39-9B16-51B95C5BDAE1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1065,183 +1161,209 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="160" zoomScaleNormal="100" zoomScaleSheetLayoutView="160" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="6.28515625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4" style="1" customWidth="1"/>
-    <col min="16" max="16" width="3.85546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5703125" style="1" customWidth="1"/>
-    <col min="18" max="18" width="6" style="1" customWidth="1"/>
-    <col min="19" max="20" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="16384" width="11.42578125" style="1" hidden="1"/>
+    <col min="3" max="3" width="26.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="7.7109375" style="1" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="3.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="4" style="1" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="3.5703125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="6" style="1" customWidth="1"/>
+    <col min="20" max="21" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="57"/>
       <c r="J1" s="27"/>
       <c r="K1" s="27"/>
-    </row>
-    <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="L1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
       <c r="B2" s="35"/>
       <c r="C2" s="36"/>
       <c r="D2" s="37"/>
       <c r="E2" s="38"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="41">
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="52">
         <v>1</v>
       </c>
-      <c r="I2" s="28"/>
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45" t="s">
+      <c r="L2" s="28"/>
+    </row>
+    <row r="3" spans="1:19" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="60" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="51">
+        <v>1</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="18"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:19" s="47" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:18" s="65" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="60" t="s">
+      <c r="B5" s="58"/>
+      <c r="C5" s="44">
+        <v>20609746387</v>
+      </c>
+      <c r="D5" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="60"/>
-      <c r="C5" s="61">
-        <v>20488089219</v>
-      </c>
-      <c r="D5" s="62" t="s">
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="44"/>
+      <c r="K5" s="44"/>
+      <c r="L5" s="46"/>
+    </row>
+    <row r="6" spans="1:19" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="43"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="54"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="46"/>
+    </row>
+    <row r="7" spans="1:19" s="5" customFormat="1" ht="21.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="45"/>
+    </row>
+    <row r="8" spans="1:19" s="5" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="64"/>
-    </row>
-    <row r="6" spans="1:18" s="5" customFormat="1" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="58"/>
-      <c r="B6" s="59"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="66"/>
-    </row>
-    <row r="7" spans="1:18" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="29" t="s">
+      <c r="B8" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C8" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D8" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="29" t="s">
+      <c r="E8" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
+      <c r="G8" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="45"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="17"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B1:G1"/>
+  <mergeCells count="8">
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B1:H1"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E5:I5"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:K4"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.12" top="0.35" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="58" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1254,7 +1376,7 @@
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1288,16 +1410,16 @@
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="56" t="s">
+      <c r="F1" s="70" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
     </row>
     <row r="2" spans="1:20" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
@@ -1315,138 +1437,138 @@
       <c r="M2" s="20"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="47" t="s">
+      <c r="B3" s="62"/>
+      <c r="C3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="26"/>
     </row>
     <row r="4" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="62"/>
+      <c r="C4" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
       <c r="M4" s="7"/>
     </row>
     <row r="5" spans="1:20" ht="33" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="55"/>
-      <c r="C5" s="57">
+      <c r="B5" s="69"/>
+      <c r="C5" s="72">
         <v>20488089219</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="G5" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
       <c r="M5" s="7"/>
     </row>
     <row r="6" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
-      <c r="B6" s="53" t="s">
+      <c r="B6" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="53" t="s">
+      <c r="D6" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="54" t="s">
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="53" t="s">
+      <c r="H6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="49" t="s">
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="49"/>
-      <c r="M6" s="52" t="s">
+      <c r="L6" s="63"/>
+      <c r="M6" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="49" t="s">
+      <c r="N6" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="49"/>
-      <c r="P6" s="52" t="s">
+      <c r="O6" s="63"/>
+      <c r="P6" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="Q6" s="49" t="s">
+      <c r="Q6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="R6" s="49"/>
-      <c r="S6" s="49"/>
-      <c r="T6" s="49"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
     </row>
     <row r="7" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="53" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53" t="s">
+      <c r="I7" s="67"/>
+      <c r="J7" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="49"/>
-      <c r="L7" s="49"/>
-      <c r="M7" s="52"/>
-      <c r="N7" s="49"/>
-      <c r="O7" s="49"/>
-      <c r="P7" s="52"/>
-      <c r="Q7" s="49"/>
-      <c r="R7" s="49"/>
-      <c r="S7" s="49"/>
-      <c r="T7" s="49"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="66"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="66"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
     </row>
     <row r="8" spans="1:20" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
       <c r="D8" s="2" t="s">
         <v>13</v>
       </c>
@@ -1456,28 +1578,28 @@
       <c r="F8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="54"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="53"/>
+      <c r="J8" s="67"/>
       <c r="K8" s="3" t="s">
         <v>18</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="M8" s="52"/>
+      <c r="M8" s="66"/>
       <c r="N8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="52"/>
+      <c r="P8" s="66"/>
       <c r="Q8" s="4" t="s">
         <v>22</v>
       </c>

</xml_diff>